<commit_message>
update rendered isotope analysis and output tables
</commit_message>
<xml_diff>
--- a/data/2017_Silverman_et_al-isotope_data_summary.xlsx
+++ b/data/2017_Silverman_et_al-isotope_data_summary.xlsx
@@ -401,10 +401,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.85848762265377</v>
+        <v>-1.12586967030865</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0258631056240202</v>
+        <v>0.0258820886792587</v>
       </c>
     </row>
     <row r="3">
@@ -421,10 +421,10 @@
         <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.05519815922711</v>
+        <v>-1.32272458888468</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0733911541653927</v>
+        <v>0.0734450219550982</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>-2.25720191491222</v>
+        <v>-1.52487661170029</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0271967152611363</v>
+        <v>0.0272166771619255</v>
       </c>
     </row>
     <row r="5">
@@ -461,10 +461,10 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.44900334135266</v>
+        <v>-1.71681881694467</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0132750348147391</v>
+        <v>0.0132847784520013</v>
       </c>
     </row>
     <row r="6">
@@ -481,10 +481,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>-2.19949805132303</v>
+        <v>-1.46713039451101</v>
       </c>
       <c r="F6" t="n">
-        <v>0.000982948312228415</v>
+        <v>0.00098366977862957</v>
       </c>
     </row>
     <row r="7">
@@ -501,10 +501,10 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>-2.30182662724558</v>
+        <v>-1.56953407777144</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0193573969967369</v>
+        <v>0.0193716049786872</v>
       </c>
     </row>
     <row r="8">
@@ -521,10 +521,10 @@
         <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.37908662212872</v>
+        <v>-1.64685078010391</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0393637679547269</v>
+        <v>0.0393926602537957</v>
       </c>
     </row>
     <row r="9">
@@ -541,10 +541,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.4648871967107</v>
+        <v>-1.73271433076741</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0302263180810171</v>
+        <v>0.0302485036558925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>